<commit_message>
Updated rubrics for total score of 40
</commit_message>
<xml_diff>
--- a/Labs/Lab06/CS133JS_Lab06_Rubric.xlsx
+++ b/Labs/Lab06/CS133JS_Lab06_Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAAFDE2-9135-5144-A3E8-CD43C1FCE27C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FBA08D-961F-4294-A899-E166F7B0BDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="1700" windowWidth="17620" windowHeight="12020" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-19212" yWindow="4308" windowWidth="17556" windowHeight="11592" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Criteria</t>
   </si>
@@ -136,12 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,15 +469,15 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D6" sqref="D6:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" customWidth="1"/>
+    <col min="3" max="3" width="36.796875" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" customWidth="1"/>
+    <col min="5" max="5" width="5.796875" customWidth="1"/>
     <col min="6" max="6" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -504,98 +514,86 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="D8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="D9">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="D12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="D13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4"/>
+      <c r="D14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="4">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4"/>
+      <c r="D15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="D16">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
@@ -603,7 +601,7 @@
       </c>
       <c r="D18">
         <f>SUM(D6:D16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -614,180 +612,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5D8D87-FF24-1E43-BB01-CA24513D1C59}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
-    <col min="6" max="6" width="1.5" customWidth="1"/>
+    <col min="1" max="1" width="39.796875" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" customWidth="1"/>
+    <col min="4" max="4" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="4">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="D18">
-        <f>SUM(D6:D16)</f>
-        <v>50</v>
-      </c>
-      <c r="E18">
-        <f>SUM(E6:E16)</f>
-        <v>50</v>
+      <c r="B18">
+        <f>SUM(B6:B16)</f>
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C6:C16)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>